<commit_message>
Added raid levels to spreadsheet.
</commit_message>
<xml_diff>
--- a/Midterm1/PerformanceCalculations.xlsx
+++ b/Midterm1/PerformanceCalculations.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pucas\Documents\Compsci\COSC 404\adv-db-code\Midterm1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC37CCAD-BD02-4826-B011-F2FA6BD9745B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EF55D5-02A2-4885-B0C1-BAD3A464BFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F2E30BBD-D36A-4256-B7D9-A683A10F4ACA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TemplateSheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -24,10 +24,47 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+  <si>
+    <t>Number of Drives</t>
+  </si>
+  <si>
+    <t>RAID</t>
+  </si>
+  <si>
+    <t>Single Drive Capacity</t>
+  </si>
+  <si>
+    <t># Parity Drives</t>
+  </si>
+  <si>
+    <t>Index calculations:</t>
+  </si>
+  <si>
+    <t>Disk block size:</t>
+  </si>
+  <si>
+    <t>Record size:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data File Size: </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -55,8 +92,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -371,12 +409,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{251F8AD5-B8A1-4C79-A2C2-2EC90D299D8A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.90625" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>8000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <f>B2*B3</f>
+        <v>64000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <f>_xlfn.CEILING.MATH(B2/2)*B3</f>
+        <v>32000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f>(B2-1)*B3</f>
+        <v>56000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f>(B2-B4)*B3</f>
+        <v>64000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>